<commit_message>
Data loader - read logic complete
</commit_message>
<xml_diff>
--- a/documents/data_model/data_sources.xlsx
+++ b/documents/data_model/data_sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\manniongeo\projects\nwfwmd\2015-01-13_gis_support\github\Hydrologic-Monitoring-Project\documents\data_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2491C500-DF75-423C-82F9-3DAC6C6348F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1EE5A5-1498-405F-A152-15B1CFBB67C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="798" activeTab="3" xr2:uid="{D4CEDCF3-9326-4FBC-A5D3-76EEC54FBE1B}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="798" firstSheet="1" activeTab="6" xr2:uid="{D4CEDCF3-9326-4FBC-A5D3-76EEC54FBE1B}"/>
   </bookViews>
   <sheets>
     <sheet name="ConductivityMeasurement" sheetId="4" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="156">
   <si>
     <t>Field Name</t>
   </si>
@@ -455,9 +455,6 @@
     <t>Recorder Serial #</t>
   </si>
   <si>
-    <t>Reference_Points_20221018.xlsx</t>
-  </si>
-  <si>
     <t>Type of Sensor</t>
   </si>
   <si>
@@ -485,9 +482,6 @@
     <t>This is the NWFID of the corresponding Location</t>
   </si>
   <si>
-    <t>Need an updated export that includes this column</t>
-  </si>
-  <si>
     <t>Source has a "Unit" column, but value always is / will be feet. On survey, add "ft" to displayed value.</t>
   </si>
   <si>
@@ -513,6 +507,20 @@
   </si>
   <si>
     <t>District Monitoring spreadsheet needs new column</t>
+  </si>
+  <si>
+    <t>Reference_Points.csv</t>
+  </si>
+  <si>
+    <t>UniqueId</t>
+  </si>
+  <si>
+    <t>Only import rows from Reference Points spreadsheet where:
+ReferencePointPeriods_0_IsMeasuredAgainstLocalAssumedDatum = "FALSE"
+Name NOT IN ("NGVD29 0ft", "NAVD88 0ft")</t>
+  </si>
+  <si>
+    <t>ReferencePointPeriods_0_Elevation</t>
   </si>
 </sst>
 </file>
@@ -585,7 +593,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -595,6 +603,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -915,10 +929,10 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection sqref="A1:D1"/>
-      <selection pane="topRight" sqref="A1:D1"/>
-      <selection pane="bottomLeft" sqref="A1:D1"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection activeCell="G9" sqref="G9"/>
+      <selection pane="topRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,8 +941,8 @@
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="50.7109375" customWidth="1"/>
+    <col min="6" max="6" width="33.7109375" customWidth="1"/>
+    <col min="7" max="7" width="80.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1039,6 +1053,7 @@
       <c r="D9" t="s">
         <v>13</v>
       </c>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1129,10 +1144,10 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection sqref="A1:D1"/>
-      <selection pane="topRight" sqref="A1:D1"/>
-      <selection pane="bottomLeft" sqref="A1:D1"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection activeCell="G9" sqref="G9"/>
+      <selection pane="topRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1141,8 +1156,8 @@
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="50.7109375" customWidth="1"/>
+    <col min="6" max="6" width="33.7109375" customWidth="1"/>
+    <col min="7" max="7" width="80.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1247,6 +1262,7 @@
       <c r="D9" t="s">
         <v>125</v>
       </c>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1293,10 +1309,10 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection sqref="A1:D1"/>
-      <selection pane="topRight" sqref="A1:D1"/>
-      <selection pane="bottomLeft" sqref="A1:D1"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection activeCell="G9" sqref="G9"/>
+      <selection pane="topRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1305,8 +1321,8 @@
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="50.7109375" customWidth="1"/>
+    <col min="6" max="6" width="33.7109375" customWidth="1"/>
+    <col min="7" max="7" width="80.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1423,6 +1439,7 @@
       <c r="D9" t="s">
         <v>131</v>
       </c>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1463,14 +1480,14 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A4E355F-95B4-441C-A1A0-3AF5195FC5EB}">
   <sheetPr codeName="Sheet13"/>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection sqref="A1:D1"/>
-      <selection pane="topRight" sqref="A1:D1"/>
-      <selection pane="bottomLeft" sqref="A1:D1"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection activeCell="G9" sqref="G9"/>
+      <selection pane="topRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1479,8 +1496,8 @@
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="50.7109375" customWidth="1"/>
+    <col min="6" max="6" width="33.7109375" customWidth="1"/>
+    <col min="7" max="7" width="80.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1539,6 +1556,9 @@
       <c r="B4" t="s">
         <v>51</v>
       </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G9" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1560,12 +1580,12 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -1580,12 +1600,12 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1596,14 +1616,14 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{097C2E08-E0AE-4E79-9515-30E93C4CF9E8}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection sqref="A1:D1"/>
-      <selection pane="topRight" sqref="A1:D1"/>
-      <selection pane="bottomLeft" sqref="A1:D1"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection activeCell="G9" sqref="G9"/>
+      <selection pane="topRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1612,8 +1632,8 @@
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="50.7109375" customWidth="1"/>
+    <col min="6" max="6" width="33.7109375" customWidth="1"/>
+    <col min="7" max="7" width="80.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1706,6 +1726,9 @@
       <c r="B6" t="s">
         <v>51</v>
       </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G9" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1728,10 +1751,10 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection sqref="A1:D1"/>
-      <selection pane="topRight" sqref="A1:D1"/>
-      <selection pane="bottomLeft" sqref="A1:D1"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection activeCell="G9" sqref="G9"/>
+      <selection pane="topRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1740,8 +1763,8 @@
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="50.7109375" customWidth="1"/>
+    <col min="6" max="6" width="33.7109375" customWidth="1"/>
+    <col min="7" max="7" width="80.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1846,6 +1869,7 @@
       <c r="D9" t="s">
         <v>13</v>
       </c>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1904,12 +1928,12 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection sqref="A1:D1"/>
-      <selection pane="topRight" sqref="A1:D1"/>
-      <selection pane="bottomLeft" sqref="A1:D1"/>
-      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
+      <selection activeCell="G9" sqref="G9"/>
+      <selection pane="topRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1918,8 +1942,8 @@
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="50.7109375" customWidth="1"/>
+    <col min="6" max="6" width="33.7109375" customWidth="1"/>
+    <col min="7" max="7" width="80.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1965,13 +1989,13 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F3" t="s">
         <v>4</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1988,10 +2012,10 @@
         <v>28</v>
       </c>
       <c r="F4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G4" t="s">
         <v>140</v>
-      </c>
-      <c r="G4" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2045,7 +2069,7 @@
         <v>32</v>
       </c>
       <c r="G7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2087,8 +2111,8 @@
       <c r="F9" t="s">
         <v>31</v>
       </c>
-      <c r="G9" t="s">
-        <v>138</v>
+      <c r="G9" s="7" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2151,12 +2175,12 @@
         <v>31</v>
       </c>
       <c r="G12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -2168,7 +2192,7 @@
         <v>13</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2259,14 +2283,14 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C21D5C8-7BA9-44F4-B641-0831C59DA9C8}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection sqref="A1:D1"/>
-      <selection pane="topRight" sqref="A1:D1"/>
-      <selection pane="bottomLeft" sqref="A1:D1"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection activeCell="G9" sqref="G9"/>
+      <selection pane="topRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2275,8 +2299,8 @@
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="50.7109375" customWidth="1"/>
+    <col min="6" max="6" width="33.7109375" customWidth="1"/>
+    <col min="7" max="7" width="80.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -2346,6 +2370,9 @@
       <c r="B5" t="s">
         <v>51</v>
       </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G9" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2369,10 +2396,10 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection sqref="A1:D1"/>
-      <selection pane="topRight" sqref="A1:D1"/>
-      <selection pane="bottomLeft" sqref="A1:D1"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection activeCell="G9" sqref="G9"/>
+      <selection pane="topRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2381,8 +2408,8 @@
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="50.7109375" customWidth="1"/>
+    <col min="6" max="6" width="33.7109375" customWidth="1"/>
+    <col min="7" max="7" width="80.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -2505,6 +2532,7 @@
       <c r="D9" t="s">
         <v>108</v>
       </c>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -2963,14 +2991,14 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F30A0A28-4805-4A16-80F5-8E4DAB824965}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection sqref="A1:D1"/>
-      <selection pane="topRight" sqref="A1:D1"/>
-      <selection pane="bottomLeft" sqref="A1:D1"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection activeCell="F2" sqref="F1:F1048576"/>
+      <selection pane="topRight" activeCell="F2" sqref="F1:F1048576"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F1:F1048576"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2979,8 +3007,8 @@
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="50.7109375" customWidth="1"/>
+    <col min="6" max="6" width="33.7109375" customWidth="1"/>
+    <col min="7" max="7" width="80.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3029,7 +3057,7 @@
         <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
@@ -3042,8 +3070,11 @@
       <c r="B4" t="s">
         <v>51</v>
       </c>
-      <c r="G4" t="s">
-        <v>144</v>
+      <c r="E4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F4" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -3057,7 +3088,7 @@
         <v>1024</v>
       </c>
       <c r="E5" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="F5" t="s">
         <v>117</v>
@@ -3071,13 +3102,13 @@
         <v>57</v>
       </c>
       <c r="E6" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="F6" t="s">
-        <v>118</v>
+        <v>155</v>
       </c>
       <c r="G6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -3099,13 +3130,18 @@
         <v>51</v>
       </c>
       <c r="E8" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="F8" t="s">
+        <v>141</v>
+      </c>
+      <c r="G8" t="s">
         <v>142</v>
       </c>
-      <c r="G8" t="s">
-        <v>143</v>
+    </row>
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G9" s="6" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -3125,14 +3161,14 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E725DF3-5C6A-456A-8EF3-79EA5D43C3AC}">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection sqref="A1:D1"/>
-      <selection pane="topRight" sqref="A1:D1"/>
-      <selection pane="bottomLeft" sqref="A1:D1"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection activeCell="G9" sqref="G9"/>
+      <selection pane="topRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3141,8 +3177,8 @@
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="50.7109375" customWidth="1"/>
+    <col min="6" max="6" width="33.7109375" customWidth="1"/>
+    <col min="7" max="7" width="80.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3217,6 +3253,9 @@
       <c r="B6" t="s">
         <v>51</v>
       </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G9" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3235,14 +3274,14 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D1E4FD-4485-41F2-8D72-C61BF926308A}">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection sqref="A1:D1"/>
-      <selection pane="topRight" sqref="A1:D1"/>
-      <selection pane="bottomLeft" sqref="A1:D1"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection activeCell="G9" sqref="G9"/>
+      <selection pane="topRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3251,8 +3290,8 @@
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="50.7109375" customWidth="1"/>
+    <col min="6" max="6" width="33.7109375" customWidth="1"/>
+    <col min="7" max="7" width="80.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3307,15 +3346,15 @@
         <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -3332,15 +3371,15 @@
         <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -3361,6 +3400,9 @@
       <c r="B8" t="s">
         <v>51</v>
       </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G9" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Data model / workflow updates
- Data model components for:
  - #74
  - #79
  - #80
  - #83
  - #84

- Closes #65
</commit_message>
<xml_diff>
--- a/documents/data_model/data_sources.xlsx
+++ b/documents/data_model/data_sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\manniongeo\projects\nwfwmd\2015-01-13_gis_support\github\Hydrologic-Monitoring-Project\documents\data_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C35103-D0FA-43F7-98B6-52A9DCD55333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8517B014-C38B-41BD-A845-03DC074AFB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="20925" tabRatio="798" activeTab="6" xr2:uid="{D4CEDCF3-9326-4FBC-A5D3-76EEC54FBE1B}"/>
+    <workbookView xWindow="1560" yWindow="210" windowWidth="29325" windowHeight="18435" tabRatio="798" activeTab="3" xr2:uid="{D4CEDCF3-9326-4FBC-A5D3-76EEC54FBE1B}"/>
   </bookViews>
   <sheets>
     <sheet name="ConductivityMeasurement" sheetId="4" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="180">
   <si>
     <t>Field Name</t>
   </si>
@@ -596,6 +596,12 @@
   </si>
   <si>
     <t>Set all values to "Yes"; all Measuring Points in source that pass validation are implicitly active</t>
+  </si>
+  <si>
+    <t>FLUID</t>
+  </si>
+  <si>
+    <t>FLUWID</t>
   </si>
 </sst>
 </file>
@@ -674,7 +680,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -685,29 +691,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1035,229 +1027,228 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" style="11" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" style="11" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" style="11" customWidth="1"/>
-    <col min="6" max="6" width="33.7109375" style="11" customWidth="1"/>
-    <col min="7" max="7" width="80.7109375" style="11" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="11"/>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="33.7109375" customWidth="1"/>
+    <col min="7" max="7" width="80.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="10" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="10"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" t="s">
         <v>98</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" s="11">
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4">
         <v>32</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" t="s">
         <v>99</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="11">
+      <c r="B5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5">
         <v>32</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" t="s">
         <v>100</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" t="s">
         <v>101</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" t="s">
         <v>102</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" t="s">
         <v>103</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="11">
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9">
         <v>3</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="15"/>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" t="s">
         <v>104</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" t="s">
         <v>105</v>
       </c>
-      <c r="B11" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" s="11">
+      <c r="B11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11">
         <v>32</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" t="s">
         <v>106</v>
       </c>
-      <c r="B12" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="C12" s="11">
+      <c r="B12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12">
         <v>1024</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="A13" t="s">
         <v>107</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" t="s">
         <v>108</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" t="s">
         <v>109</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" t="s">
         <v>108</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" t="s">
         <v>110</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="A16" t="s">
         <v>111</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="A17" t="s">
         <v>112</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1306,16 +1297,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="7"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1341,133 +1332,133 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" t="s">
         <v>101</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" t="s">
         <v>102</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" t="s">
         <v>103</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" t="s">
         <v>83</v>
       </c>
       <c r="C8">
         <v>3</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" t="s">
         <v>81</v>
       </c>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" t="s">
         <v>105</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" t="s">
         <v>83</v>
       </c>
       <c r="C10">
         <v>32</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" t="s">
         <v>106</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" t="s">
         <v>83</v>
       </c>
       <c r="C11">
         <v>1024</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" t="s">
         <v>112</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" t="s">
         <v>116</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1516,16 +1507,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="7"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1551,103 +1542,103 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" t="s">
         <v>98</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" t="s">
         <v>83</v>
       </c>
       <c r="C4">
         <v>32</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" t="s">
         <v>99</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" t="s">
         <v>83</v>
       </c>
       <c r="C5">
         <v>32</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" t="s">
         <v>100</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" t="s">
         <v>101</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" t="s">
         <v>172</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" t="s">
         <v>83</v>
       </c>
       <c r="C8">
         <v>32</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" t="s">
         <v>173</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" t="s">
         <v>83</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" t="s">
         <v>10</v>
       </c>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" t="s">
         <v>112</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1684,8 +1675,8 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="B4" activeCellId="1" sqref="B2 B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1874,16 +1865,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="7"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1909,16 +1900,16 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" t="s">
         <v>113</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" t="s">
         <v>83</v>
       </c>
       <c r="C3">
         <v>64</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" t="s">
         <v>30</v>
       </c>
       <c r="E3" t="s">
@@ -1929,16 +1920,16 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" t="s">
         <v>99</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" t="s">
         <v>83</v>
       </c>
       <c r="C4">
         <v>32</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" t="s">
         <v>81</v>
       </c>
       <c r="E4" t="s">
@@ -1949,27 +1940,27 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" t="s">
         <v>83</v>
       </c>
       <c r="C5">
         <v>1024</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" t="s">
         <v>114</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2021,16 +2012,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="7"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2056,147 +2047,147 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" t="s">
         <v>98</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" t="s">
         <v>83</v>
       </c>
       <c r="C4">
         <v>32</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" t="s">
         <v>101</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" t="s">
         <v>102</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" t="s">
         <v>103</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" t="s">
         <v>83</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" t="s">
         <v>10</v>
       </c>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" t="s">
         <v>104</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" t="s">
         <v>105</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" t="s">
         <v>83</v>
       </c>
       <c r="C11">
         <v>32</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" t="s">
         <v>106</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" t="s">
         <v>83</v>
       </c>
       <c r="C12">
         <v>1024</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" t="s">
         <v>112</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" t="s">
         <v>116</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2223,14 +2214,14 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA1630B-69B0-4285-ACAD-F3C5FE33A42B}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection sqref="A1:D1"/>
       <selection pane="topRight" sqref="A1:D1"/>
       <selection pane="bottomLeft" sqref="A1:D1"/>
-      <selection pane="bottomRight" sqref="A1:D1"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2245,16 +2236,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="7"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2280,13 +2271,13 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" t="s">
         <v>81</v>
       </c>
       <c r="E3" t="s">
@@ -2295,21 +2286,21 @@
       <c r="F3" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" t="s">
         <v>83</v>
       </c>
       <c r="C4">
         <v>6</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" t="s">
         <v>81</v>
       </c>
       <c r="E4" t="s">
@@ -2323,16 +2314,16 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" t="s">
         <v>83</v>
       </c>
       <c r="C5">
         <v>128</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" t="s">
         <v>81</v>
       </c>
       <c r="E5" t="s">
@@ -2343,13 +2334,13 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" t="s">
         <v>81</v>
       </c>
       <c r="E6" t="s">
@@ -2360,59 +2351,58 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="10">
+        <v>16</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" t="s">
         <v>83</v>
       </c>
       <c r="C8">
         <v>3</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" t="s">
         <v>10</v>
       </c>
       <c r="E8" t="s">
         <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="G8" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="B9" s="8" t="s">
+      <c r="A9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" t="s">
         <v>83</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" t="s">
         <v>10</v>
       </c>
       <c r="E9" t="s">
@@ -2421,21 +2411,18 @@
       <c r="F9" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="B10" s="8" t="s">
+      <c r="A10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" t="s">
         <v>83</v>
       </c>
       <c r="C10">
         <v>3</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" t="s">
         <v>10</v>
       </c>
       <c r="E10" t="s">
@@ -2444,18 +2431,21 @@
       <c r="F10" t="s">
         <v>20</v>
       </c>
+      <c r="G10" s="5" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B11" s="8" t="s">
+      <c r="A11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" t="s">
         <v>83</v>
       </c>
       <c r="C11">
         <v>3</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" t="s">
         <v>10</v>
       </c>
       <c r="E11" t="s">
@@ -2466,16 +2456,16 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12" s="8" t="s">
+      <c r="A12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" t="s">
         <v>83</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" t="s">
         <v>10</v>
       </c>
       <c r="E12" t="s">
@@ -2484,58 +2474,58 @@
       <c r="F12" t="s">
         <v>20</v>
       </c>
-      <c r="G12" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="B13" s="8" t="s">
+      <c r="A13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" t="s">
         <v>83</v>
       </c>
       <c r="C13">
         <v>3</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>73</v>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B14" s="8" t="s">
+      <c r="A14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" t="s">
         <v>83</v>
       </c>
       <c r="C14">
         <v>3</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" t="s">
         <v>10</v>
       </c>
-      <c r="E14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" t="s">
-        <v>20</v>
+      <c r="G14" s="3" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="B15" s="8" t="s">
+      <c r="A15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" t="s">
         <v>83</v>
       </c>
       <c r="C15">
         <v>3</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" t="s">
         <v>10</v>
       </c>
       <c r="E15" t="s">
@@ -2546,16 +2536,16 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B16" s="8" t="s">
+      <c r="A16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" t="s">
         <v>83</v>
       </c>
       <c r="C16">
         <v>3</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" t="s">
         <v>10</v>
       </c>
       <c r="E16" t="s">
@@ -2565,17 +2555,37 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>96</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C17">
+      <c r="B18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18">
         <v>1024</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D18" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2585,13 +2595,13 @@
     <mergeCell ref="E1:F1"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E100" xr:uid="{E14B8CFD-252E-4BEE-8954-B715D6F74475}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E101" xr:uid="{E14B8CFD-252E-4BEE-8954-B715D6F74475}">
       <formula1>SourceTables</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D100" xr:uid="{50AEDC82-750E-4AB2-B988-5BA28F1D7EA2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D101" xr:uid="{50AEDC82-750E-4AB2-B988-5BA28F1D7EA2}">
       <formula1>Domains</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B100" xr:uid="{A3E3D7D2-77C6-45BC-9259-8E156A892B39}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B101" xr:uid="{A3E3D7D2-77C6-45BC-9259-8E156A892B39}">
       <formula1>DataTypes</formula1>
     </dataValidation>
   </dataValidations>
@@ -2624,16 +2634,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="7"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2740,16 +2750,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="7"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2775,721 +2785,721 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" t="s">
         <v>117</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" t="s">
         <v>118</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" t="s">
         <v>83</v>
       </c>
       <c r="C4">
         <v>1024</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" t="s">
         <v>119</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" t="s">
         <v>83</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" t="s">
         <v>120</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" t="s">
         <v>83</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" t="s">
         <v>121</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" t="s">
         <v>83</v>
       </c>
       <c r="C7">
         <v>32</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" t="s">
         <v>122</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" t="s">
         <v>123</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" t="s">
         <v>83</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" t="s">
         <v>10</v>
       </c>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" t="s">
         <v>124</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" t="s">
         <v>125</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" t="s">
         <v>83</v>
       </c>
       <c r="C11">
         <v>32</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" t="s">
         <v>126</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" t="s">
         <v>83</v>
       </c>
       <c r="C12">
         <v>1024</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" t="s">
         <v>127</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" t="s">
         <v>83</v>
       </c>
       <c r="C13">
         <v>32</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" t="s">
         <v>128</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" t="s">
         <v>83</v>
       </c>
       <c r="C14">
         <v>32</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" t="s">
         <v>129</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" t="s">
         <v>83</v>
       </c>
       <c r="C15">
         <v>32</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="A16" t="s">
         <v>130</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" t="s">
         <v>83</v>
       </c>
       <c r="C16">
         <v>1024</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="A17" t="s">
         <v>131</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="A18" t="s">
         <v>132</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="A19" t="s">
         <v>133</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" t="s">
         <v>83</v>
       </c>
       <c r="C19">
         <v>32</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+      <c r="A20" t="s">
         <v>134</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+      <c r="A21" t="s">
         <v>135</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+      <c r="A22" t="s">
         <v>136</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" t="s">
         <v>83</v>
       </c>
       <c r="C22">
         <v>3</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+      <c r="A23" t="s">
         <v>137</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" t="s">
         <v>83</v>
       </c>
       <c r="C23">
         <v>32</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="A24" t="s">
         <v>138</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" t="s">
         <v>83</v>
       </c>
       <c r="C24">
         <v>1024</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+      <c r="A25" t="s">
         <v>139</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" t="s">
         <v>83</v>
       </c>
       <c r="C25">
         <v>3</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="A26" t="s">
         <v>140</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" t="s">
         <v>83</v>
       </c>
       <c r="C26">
         <v>32</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+      <c r="A27" t="s">
         <v>141</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" t="s">
         <v>83</v>
       </c>
       <c r="C27">
         <v>1024</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+      <c r="A28" t="s">
         <v>142</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" t="s">
         <v>83</v>
       </c>
       <c r="C28">
         <v>3</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+      <c r="A29" t="s">
         <v>143</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" t="s">
         <v>83</v>
       </c>
       <c r="C29">
         <v>32</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+      <c r="A30" t="s">
         <v>144</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" t="s">
         <v>31</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
+      <c r="A31" t="s">
         <v>145</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" t="s">
         <v>83</v>
       </c>
       <c r="C31">
         <v>3</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
+      <c r="A32" t="s">
         <v>146</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" t="s">
         <v>12</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+      <c r="A33" t="s">
         <v>147</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" t="s">
         <v>83</v>
       </c>
       <c r="C33">
         <v>32</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
+      <c r="A34" t="s">
         <v>148</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" t="s">
         <v>83</v>
       </c>
       <c r="C34">
         <v>1024</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
+      <c r="A35" t="s">
         <v>149</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" t="s">
         <v>12</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+      <c r="A36" t="s">
         <v>150</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" t="s">
         <v>12</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
+      <c r="A37" t="s">
         <v>151</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" t="s">
         <v>83</v>
       </c>
       <c r="C37">
         <v>3</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
+      <c r="A38" t="s">
         <v>152</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" t="s">
         <v>83</v>
       </c>
       <c r="C38">
         <v>32</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
+      <c r="A39" t="s">
         <v>153</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" t="s">
         <v>83</v>
       </c>
       <c r="C39">
         <v>1024</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
+      <c r="A40" t="s">
         <v>154</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" t="s">
         <v>83</v>
       </c>
       <c r="C40">
         <v>3</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D40" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
+      <c r="A41" t="s">
         <v>155</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B41" t="s">
         <v>83</v>
       </c>
       <c r="C41">
         <v>32</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D41" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
+      <c r="A42" t="s">
         <v>156</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B42" t="s">
         <v>83</v>
       </c>
       <c r="C42">
         <v>1024</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D42" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
+      <c r="A43" t="s">
         <v>157</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B43" t="s">
         <v>83</v>
       </c>
       <c r="C43">
         <v>3</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
+      <c r="A44" t="s">
         <v>158</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B44" t="s">
         <v>83</v>
       </c>
       <c r="C44">
         <v>32</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="D44" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
+      <c r="A45" t="s">
         <v>159</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B45" t="s">
         <v>83</v>
       </c>
       <c r="C45">
         <v>1024</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D45" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="s">
+      <c r="A46" t="s">
         <v>160</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B46" t="s">
         <v>83</v>
       </c>
       <c r="C46">
         <v>32</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D46" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="s">
+      <c r="A47" t="s">
         <v>161</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" t="s">
         <v>12</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D47" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="s">
+      <c r="A48" t="s">
         <v>162</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B48" t="s">
         <v>12</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="D48" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="8" t="s">
+      <c r="A49" t="s">
         <v>163</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B49" t="s">
         <v>12</v>
       </c>
-      <c r="D49" s="8" t="s">
+      <c r="D49" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
+      <c r="A50" t="s">
         <v>164</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B50" t="s">
         <v>12</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="D50" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
+      <c r="A51" t="s">
         <v>165</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B51" t="s">
         <v>31</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="D51" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
+      <c r="A52" t="s">
         <v>166</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B52" t="s">
         <v>31</v>
       </c>
-      <c r="D52" s="8" t="s">
+      <c r="D52" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
+      <c r="A53" t="s">
         <v>167</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B53" t="s">
         <v>83</v>
       </c>
       <c r="C53">
         <v>3</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="D53" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="8" t="s">
+      <c r="A54" t="s">
         <v>168</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="B54" t="s">
         <v>12</v>
       </c>
-      <c r="D54" s="8" t="s">
+      <c r="D54" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="8" t="s">
+      <c r="A55" t="s">
         <v>169</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B55" t="s">
         <v>12</v>
       </c>
-      <c r="D55" s="8" t="s">
+      <c r="D55" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="8" t="s">
+      <c r="A56" t="s">
         <v>170</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B56" t="s">
         <v>12</v>
       </c>
-      <c r="D56" s="8" t="s">
+      <c r="D56" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="8" t="s">
+      <c r="A57" t="s">
         <v>171</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="B57" t="s">
         <v>12</v>
       </c>
-      <c r="D57" s="8" t="s">
+      <c r="D57" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="8" t="s">
+      <c r="A58" t="s">
         <v>114</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="B58" t="s">
         <v>28</v>
       </c>
-      <c r="D58" s="8" t="s">
+      <c r="D58" t="s">
         <v>81</v>
       </c>
     </row>
@@ -3518,7 +3528,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection sqref="A1:D1"/>
       <selection pane="topRight" sqref="A1:D1"/>
@@ -3538,16 +3548,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="7"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -3650,8 +3660,8 @@
       <c r="D7" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="18" t="s">
+      <c r="E7" s="6"/>
+      <c r="F7" s="7" t="s">
         <v>176</v>
       </c>
       <c r="G7" t="s">
@@ -3736,16 +3746,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="7"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -3856,16 +3866,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="7"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">

</xml_diff>